<commit_message>
He empezado a arreglar los errores entre Anfígenos halógenos
</commit_message>
<xml_diff>
--- a/Hojas de Calculo/anfigenoshalogenos.xlsx
+++ b/Hojas de Calculo/anfigenoshalogenos.xlsx
@@ -171,12 +171,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
He añadido los elementos de las sales volátiles (N, P, As, Si,...) a la hoja de cálculo de Anfígenos y Halógenos
</commit_message>
<xml_diff>
--- a/Hojas de Calculo/anfigenoshalogenos.xlsx
+++ b/Hojas de Calculo/anfigenoshalogenos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Nuevo_Nombre_Elemento</t>
   </si>
@@ -62,6 +62,42 @@
   </si>
   <si>
     <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siliciuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carburo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitruro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fosfuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arseniuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boruro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B </t>
   </si>
 </sst>
 </file>
@@ -142,12 +178,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,13 +208,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
   </cols>
@@ -187,7 +227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -195,7 +235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -203,7 +243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -211,7 +251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -219,7 +259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -233,6 +273,54 @@
       </c>
       <c r="B7" s="0" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>